<commit_message>
1. Add the description about function point "extract value from single cell". 2. Add some test case about the above function point.
Signed-off-by: Spark-Liang <369453502@qq.com>
</commit_message>
<xml_diff>
--- a/test/xl_transform/reader_test/test_data/CellValueExtractor/CanReadSingleCellWithTypehints/Source.xlsx
+++ b/test/xl_transform/reader_test/test_data/CellValueExtractor/CanReadSingleCellWithTypehints/Source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\ProjectData\ExcelTransformer\test\xl_transform\reader_test\test_data\DataFrameReader\CanReadSingleCellWithTypehints\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\ProjectData\ExcelTransformer\test\xl_transform\reader_test\test_data\CellValueExtractor\CanReadSingleCellWithTypehints\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,10 +16,6 @@
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -941,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B4"/>
+  <dimension ref="A2:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -965,6 +961,11 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B4" s="2"/>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B6" s="2">
+        <v>43822</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>